<commit_message>
Archivo con actualizaciónes durante el desarrollo
</commit_message>
<xml_diff>
--- a/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
+++ b/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26920"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D80A7C-6B6A-491C-AB30-680F3765FF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Alcance" sheetId="4" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <sheet name="Supuestos" sheetId="11" r:id="rId5"/>
     <sheet name="Bugs" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="131">
   <si>
     <t>Alcance</t>
   </si>
@@ -455,12 +454,18 @@
       <t xml:space="preserve"> No se encontraron más bugs. Ya que es una página profesional en producción.</t>
     </r>
   </si>
+  <si>
+    <t>  No</t>
+  </si>
+  <si>
+    <t>Sebastian Vasquez</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1226,11 +1231,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1344,57 +1350,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1516,9 +1471,64 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1554,7 +1564,7 @@
         <xdr:cNvPr id="12" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,10 +1666,10 @@
         <xdr:cNvPr id="77" name="CuadroTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1815,10 +1825,10 @@
         <xdr:cNvPr id="26" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,10 +1984,10 @@
         <xdr:cNvPr id="19" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,10 +2166,10 @@
         <xdr:cNvPr id="23" name="CuadroTexto 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2338,10 +2348,10 @@
         <xdr:cNvPr id="2" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2562,10 +2572,10 @@
         <xdr:cNvPr id="41" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2760,10 +2770,10 @@
         <xdr:cNvPr id="15" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2919,10 +2929,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,10 +3101,10 @@
         <xdr:cNvPr id="5" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3260,10 +3270,10 @@
         <xdr:cNvPr id="16" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3445,10 +3455,10 @@
         <xdr:cNvPr id="7" name="CuadroTexto 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3630,10 +3640,10 @@
         <xdr:cNvPr id="21" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3866,10 +3876,10 @@
         <xdr:cNvPr id="75" name="CuadroTexto 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4136,10 +4146,10 @@
         <xdr:cNvPr id="37" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4291,7 +4301,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> Register successful</a:t>
+            <a:t> Invalid successful</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -4332,7 +4342,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
               <a:solidFill>
@@ -4351,45 +4360,17 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> The user enters the credentials</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>And</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>: Confirm password</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The user enters the incorrect data</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
@@ -4436,10 +4417,10 @@
         <xdr:cNvPr id="60" name="CuadroTexto 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5056,10 +5037,10 @@
         <xdr:cNvPr id="42" name="CuadroTexto 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5326,10 +5307,10 @@
         <xdr:cNvPr id="53" name="CuadroTexto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5596,10 +5577,10 @@
         <xdr:cNvPr id="55" name="CuadroTexto 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5866,10 +5847,10 @@
         <xdr:cNvPr id="72" name="CuadroTexto 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6136,10 +6117,10 @@
         <xdr:cNvPr id="43" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6436,10 +6417,10 @@
         <xdr:cNvPr id="64" name="CuadroTexto 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6736,10 +6717,10 @@
         <xdr:cNvPr id="65" name="CuadroTexto 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7036,10 +7017,10 @@
         <xdr:cNvPr id="73" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7341,7 +7322,7 @@
         <xdr:cNvPr id="3" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7385,10 +7366,10 @@
         <xdr:cNvPr id="10" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7474,10 +7455,10 @@
         <xdr:cNvPr id="2" name="Conector recto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7532,10 +7513,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7731,10 +7712,10 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7806,7 +7787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -7858,7 +7839,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -8052,27 +8033,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DAC4AF-3F9A-4271-9B0B-277FBE221652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="23.25" customHeight="1">
+    <row r="2" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8080,60 +8061,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="60.75" customHeight="1">
+    <row r="3" spans="2:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="90" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15" customHeight="1">
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="50"/>
+      <c r="C4" s="90"/>
     </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1">
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="90"/>
     </row>
-    <row r="6" spans="2:3" ht="15" customHeight="1">
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="90"/>
     </row>
-    <row r="7" spans="2:3" ht="15" customHeight="1">
+    <row r="7" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="90"/>
     </row>
-    <row r="8" spans="2:3" ht="15" customHeight="1">
+    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="50"/>
+      <c r="C8" s="90"/>
     </row>
-    <row r="9" spans="2:3" ht="15" customHeight="1">
+    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="50"/>
+      <c r="C9" s="90"/>
     </row>
-    <row r="10" spans="2:3" ht="15" customHeight="1">
+    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="90"/>
     </row>
-    <row r="11" spans="2:3" ht="27.75" customHeight="1">
+    <row r="11" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="91"/>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1"/>
-    <row r="13" spans="2:3" ht="15" customHeight="1"/>
-    <row r="14" spans="2:3" ht="13.5" customHeight="1"/>
-    <row r="15" spans="2:3" ht="15" customHeight="1"/>
-    <row r="16" spans="2:3" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:C11"/>
@@ -8143,113 +8124,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D14B542-D681-42FB-AEEB-27F195955836}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="140.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="53"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="93"/>
       <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="53"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="93"/>
       <c r="C4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B5" s="53"/>
+    <row r="5" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="93"/>
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="53"/>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="93"/>
       <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="53"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="93"/>
       <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="53"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="93"/>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="53"/>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="93"/>
       <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30" customHeight="1">
-      <c r="B10" s="53"/>
+    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="93"/>
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B11" s="53"/>
+    <row r="11" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="93"/>
       <c r="C11" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1">
-      <c r="B12" s="53"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="93"/>
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="53"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="93"/>
       <c r="C13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="53"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="93"/>
       <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B15" s="53"/>
+    <row r="15" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="93"/>
       <c r="C15" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="16.5" customHeight="1">
-      <c r="B16" s="53"/>
+    <row r="16" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="93"/>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B17" s="54"/>
+    <row r="17" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="94"/>
       <c r="C17" s="16" t="s">
         <v>24</v>
       </c>
@@ -8263,14 +8244,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="G5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
@@ -8282,217 +8263,217 @@
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.25" customHeight="1">
-      <c r="B2" s="103" t="s">
+    <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="104" t="s">
+      <c r="K2" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="88" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="107.25" customHeight="1">
-      <c r="B3" s="92" t="s">
+    <row r="3" spans="2:12" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="102" t="s">
+      <c r="I3" s="84"/>
+      <c r="J3" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="126.75" customHeight="1">
-      <c r="B4" s="96" t="s">
+    <row r="4" spans="2:12" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="H4" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="106" t="s">
+      <c r="K4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="100" t="s">
+      <c r="L4" s="83" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="111.75" customHeight="1">
-      <c r="B5" s="92" t="s">
+    <row r="5" spans="2:12" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="83" t="s">
+      <c r="K5" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="112.5" customHeight="1">
-      <c r="B6" s="96" t="s">
+    <row r="6" spans="2:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="99" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="100" t="s">
+      <c r="K6" s="82" t="s">
+        <v>130</v>
+      </c>
+      <c r="L6" s="83" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="127.5" customHeight="1">
-      <c r="B7" s="92" t="s">
+    <row r="7" spans="2:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" s="71" t="s">
-        <v>51</v>
+      <c r="K7" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="54" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="223.5" customHeight="1">
-      <c r="B8" s="89" t="s">
+    <row r="8" spans="2:12" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="34" t="s">
@@ -8510,59 +8491,59 @@
       <c r="H8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="86" t="s">
+      <c r="I8" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="117.75" customHeight="1">
-      <c r="B9" s="87" t="s">
+    <row r="9" spans="2:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="106.5" customHeight="1">
-      <c r="B10" s="89" t="s">
+    <row r="10" spans="2:12" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D10" s="34" t="s">
@@ -8580,59 +8561,59 @@
       <c r="H10" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="100.5" customHeight="1">
-      <c r="B11" s="87" t="s">
+    <row r="11" spans="2:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="76" t="s">
+      <c r="G11" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="80" t="s">
+      <c r="K11" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="81" t="s">
+      <c r="L11" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="111" customHeight="1">
-      <c r="B12" s="89" t="s">
+    <row r="12" spans="2:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="34" t="s">
@@ -8650,59 +8631,59 @@
       <c r="H12" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="86" t="s">
+      <c r="I12" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="K12" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="131.25" customHeight="1">
-      <c r="B13" s="87" t="s">
+    <row r="13" spans="2:12" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="80" t="s">
+      <c r="K13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="64" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="118.5" customHeight="1">
-      <c r="B14" s="89" t="s">
+    <row r="14" spans="2:12" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="73" t="s">
         <v>91</v>
       </c>
       <c r="D14" s="34" t="s">
@@ -8720,136 +8701,139 @@
       <c r="H14" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="86" t="s">
+      <c r="I14" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="73" t="s">
+      <c r="K14" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="57" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9456DD7-BBEC-42B0-AB3D-1E4232459D96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="58"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="98"/>
       <c r="C3" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="58"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="98"/>
       <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="58"/>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
       <c r="C5" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="58"/>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="98"/>
       <c r="C6" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="58"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="98"/>
       <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="58"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="98"/>
       <c r="C8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="58"/>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="98"/>
       <c r="C9" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B10" s="58"/>
+    <row r="10" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="98"/>
       <c r="C10" s="45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="59"/>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="99"/>
       <c r="C11" s="46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B12" s="55" t="s">
+    <row r="12" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="95" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B13" s="60"/>
+    <row r="13" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="100"/>
       <c r="C13" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B14" s="56"/>
+    <row r="14" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96"/>
       <c r="C14" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="55" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="95" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="96"/>
       <c r="C16" s="44" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B15:B16"/>
@@ -8861,48 +8845,48 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4F0DA6-9A0E-4C2E-8A4F-0A607ED1017F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="26.25" customHeight="1"/>
-    <row r="2" spans="2:3" ht="18" customHeight="1">
-      <c r="B2" s="61" t="s">
+    <row r="1" spans="2:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="101" t="s">
         <v>115</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="62"/>
+    <row r="3" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="102"/>
       <c r="C3" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1">
-      <c r="B4" s="63"/>
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="103"/>
       <c r="C4" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="29.25" customHeight="1">
-      <c r="B5" s="64"/>
+    <row r="5" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="104"/>
       <c r="C5" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="18.75" customHeight="1">
+    <row r="6" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>120</v>
       </c>
@@ -8919,14 +8903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3699CD-5D7B-4491-8CD4-CAE8F382A34A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
@@ -8935,7 +8919,7 @@
     <col min="6" max="6" width="124.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>25</v>
       </c>
@@ -8952,7 +8936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="159" customHeight="1">
+    <row r="3" spans="2:6" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41">
         <v>1</v>
       </c>
@@ -8965,7 +8949,7 @@
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="2:6" ht="150" customHeight="1">
+    <row r="4" spans="2:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42">
         <v>2</v>
       </c>
@@ -8978,53 +8962,53 @@
       <c r="E4" s="21"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
     </row>
-    <row r="12" spans="2:6" ht="183" customHeight="1">
-      <c r="B12" s="65" t="s">
+    <row r="12" spans="2:6" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Casos de prueba actualizados durante el desarrollo
</commit_message>
<xml_diff>
--- a/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
+++ b/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26920"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D80A7C-6B6A-491C-AB30-680F3765FF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Alcance" sheetId="4" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <sheet name="Supuestos" sheetId="11" r:id="rId5"/>
     <sheet name="Bugs" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="133">
   <si>
     <t>Alcance</t>
   </si>
@@ -455,12 +454,24 @@
       <t xml:space="preserve"> No se encontraron más bugs. Ya que es una página profesional en producción.</t>
     </r>
   </si>
+  <si>
+    <t>Validar que al momento de dar clic en el filtro de mas bajo precio si de un resultado de valore de menor a mayor</t>
+  </si>
+  <si>
+    <t>Se debera mostrar el boton para filtrar el precio mas bajo</t>
+  </si>
+  <si>
+    <t> Se visualiza el boton exitosamente</t>
+  </si>
+  <si>
+    <t> 05</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1225,12 +1236,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1344,57 +1370,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1516,9 +1491,63 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1554,7 +1583,7 @@
         <xdr:cNvPr id="12" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,10 +1685,10 @@
         <xdr:cNvPr id="77" name="CuadroTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1815,10 +1844,10 @@
         <xdr:cNvPr id="26" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,10 +2003,10 @@
         <xdr:cNvPr id="19" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,10 +2185,10 @@
         <xdr:cNvPr id="23" name="CuadroTexto 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2323,7 +2352,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>202406</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>590550</xdr:rowOff>
     </xdr:from>
@@ -2331,17 +2360,17 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>4105275</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2162175</xdr:rowOff>
+      <xdr:rowOff>2571750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2349,8 +2378,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7772400" y="8620125"/>
-          <a:ext cx="4105275" cy="1571625"/>
+          <a:off x="7965281" y="8615363"/>
+          <a:ext cx="3902869" cy="1981200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2562,10 +2591,10 @@
         <xdr:cNvPr id="41" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2760,10 +2789,10 @@
         <xdr:cNvPr id="15" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2919,10 +2948,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,10 +3120,10 @@
         <xdr:cNvPr id="5" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3260,10 +3289,10 @@
         <xdr:cNvPr id="16" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3445,10 +3474,10 @@
         <xdr:cNvPr id="7" name="CuadroTexto 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3630,10 +3659,10 @@
         <xdr:cNvPr id="21" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3866,10 +3895,10 @@
         <xdr:cNvPr id="75" name="CuadroTexto 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4136,10 +4165,10 @@
         <xdr:cNvPr id="37" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4436,10 +4465,10 @@
         <xdr:cNvPr id="60" name="CuadroTexto 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4534,505 +4563,411 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Feature:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Accommodation</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Scenario Outline</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Search hotel deals with params and filters</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-CO"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Given</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user gets into the accommodation page</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user changes the currency</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters destination name params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters in and out date params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters the person params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user performs a search at accommodation page</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user filters by stars</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user filters by price</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>the user orders by price</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters in the hotel offers</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Then</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can the the apllied params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>And</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can see the applied filters</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Scenario:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Search hotel deals with params and filters</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Given:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user gets into the accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user changes the currency</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters destination name params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user enters in and out date params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters the person params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>: The user performs a search at accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user filters by stars</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user filters by price</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> the user orders by price</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters in the hotel offers</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Then: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user can the the apllied params </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>   And:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user can see the applied filters</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5056,10 +4991,10 @@
         <xdr:cNvPr id="42" name="CuadroTexto 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5326,10 +5261,10 @@
         <xdr:cNvPr id="53" name="CuadroTexto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5596,10 +5531,10 @@
         <xdr:cNvPr id="55" name="CuadroTexto 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5866,10 +5801,10 @@
         <xdr:cNvPr id="72" name="CuadroTexto 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6136,10 +6071,10 @@
         <xdr:cNvPr id="43" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6234,185 +6169,169 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Feature:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Accommodation</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Scenario</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Search hotel deals with params and filters</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Given</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user gets into the accommodation page</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user changes the currency</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters the person params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Then</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can see a age select for each kid</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Scenario:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Search hotel deals with params and filters</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Given:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user gets into the accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters the person params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Then: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user can see a age select for each kid</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6428,18 +6347,18 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>4438650</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1309687</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="64" name="CuadroTexto 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6447,8 +6366,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15868650" y="12496800"/>
-          <a:ext cx="4238625" cy="1152525"/>
+          <a:off x="15868650" y="12492038"/>
+          <a:ext cx="4238625" cy="1176337"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6534,185 +6453,151 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Feature:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Accommodation</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Scenario</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Search hotel deals with params and filters</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Given </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user gets into the accommodation page</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user changes the currency</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user performs a search at accommodation page</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Then </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can see the destion required popup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Scenario:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Search hotel deals with params and filters</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Given:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user gets into the accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>: The user performs a search at accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Then: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user can see the destion required popup</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6721,25 +6606,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>214312</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>145256</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4429125</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>4452937</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1178719</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="65" name="CuadroTexto 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6747,8 +6632,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15859125" y="13754100"/>
-          <a:ext cx="4238625" cy="1238250"/>
+          <a:off x="15882937" y="13861256"/>
+          <a:ext cx="4238625" cy="1033463"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6834,185 +6719,152 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Feature:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> Accommodation</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Scenario</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>: Max person params values</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Given</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user gets into the accommodation page</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user changes the currency</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user enters max params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Then</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can see that the person params buttons are disabled</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Scenario:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>  Max person params values</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Given:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user gets into the accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters the person params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Then: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user can see that the person params buttons are disabled</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7036,10 +6888,10 @@
         <xdr:cNvPr id="73" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7134,6 +6986,471 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
           <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Scenario</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>: Min person params values</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Given</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user gets into the accommodation page</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user changes the currency</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>When</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user just deploys person Params</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200" b="1">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Then</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1200">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The user can see that the person minimun params buttons are disabled</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4133850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1476375</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="CuadroTexto 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7791450" y="19933444"/>
+          <a:ext cx="4105275" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>1. Ingresar a la pagina web "www.booking.com".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2. Dar click en el apartado de "Atracciones Turisticas" .</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>3. Ingresar la ciudad a visitar.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>4.Ingresar la fecha</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>5. Hacer click en el botón "Buscar" </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>6. Hacer click en el el botón "Precio mas bajo"</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3800475</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1485900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="CuadroTexto 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15716250" y="18061781"/>
+          <a:ext cx="3752850" cy="1485900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr spcFirstLastPara="0" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
@@ -7151,7 +7468,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> Accommodation</a:t>
+            <a:t> Tourist Atracttions</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7172,146 +7489,65 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Scenario:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>  Min person params values</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Given:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user gets into the accommodation page</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>When:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> The user enters the person params</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Then: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The user can see that the person params buttons are disabled</a:t>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Given The user gets into the tourist atracttions</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>When The user performs a search</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>And The user sort by price</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Then The user can see the price from low to high</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7341,7 +7577,7 @@
         <xdr:cNvPr id="3" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7385,10 +7621,10 @@
         <xdr:cNvPr id="10" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7474,10 +7710,10 @@
         <xdr:cNvPr id="2" name="Conector recto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7532,10 +7768,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7731,10 +7967,10 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7806,7 +8042,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -7858,7 +8094,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -8052,27 +8288,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DAC4AF-3F9A-4271-9B0B-277FBE221652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="23.25" customHeight="1">
+    <row r="2" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8080,60 +8316,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="60.75" customHeight="1">
+    <row r="3" spans="2:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="90" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15" customHeight="1">
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="50"/>
+      <c r="C4" s="90"/>
     </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1">
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="90"/>
     </row>
-    <row r="6" spans="2:3" ht="15" customHeight="1">
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="90"/>
     </row>
-    <row r="7" spans="2:3" ht="15" customHeight="1">
+    <row r="7" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="90"/>
     </row>
-    <row r="8" spans="2:3" ht="15" customHeight="1">
+    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="50"/>
+      <c r="C8" s="90"/>
     </row>
-    <row r="9" spans="2:3" ht="15" customHeight="1">
+    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="50"/>
+      <c r="C9" s="90"/>
     </row>
-    <row r="10" spans="2:3" ht="15" customHeight="1">
+    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="90"/>
     </row>
-    <row r="11" spans="2:3" ht="27.75" customHeight="1">
+    <row r="11" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="91"/>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1"/>
-    <row r="13" spans="2:3" ht="15" customHeight="1"/>
-    <row r="14" spans="2:3" ht="13.5" customHeight="1"/>
-    <row r="15" spans="2:3" ht="15" customHeight="1"/>
-    <row r="16" spans="2:3" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:C11"/>
@@ -8143,113 +8379,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D14B542-D681-42FB-AEEB-27F195955836}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="140.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="53"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="93"/>
       <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="53"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="93"/>
       <c r="C4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B5" s="53"/>
+    <row r="5" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="93"/>
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="53"/>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="93"/>
       <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="53"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="93"/>
       <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="53"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="93"/>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="53"/>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="93"/>
       <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30" customHeight="1">
-      <c r="B10" s="53"/>
+    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="93"/>
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B11" s="53"/>
+    <row r="11" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="93"/>
       <c r="C11" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1">
-      <c r="B12" s="53"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="93"/>
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="53"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="93"/>
       <c r="C13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="53"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="93"/>
       <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B15" s="53"/>
+    <row r="15" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="93"/>
       <c r="C15" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="16.5" customHeight="1">
-      <c r="B16" s="53"/>
+    <row r="16" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="93"/>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B17" s="54"/>
+    <row r="17" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="94"/>
       <c r="C17" s="16" t="s">
         <v>24</v>
       </c>
@@ -8263,14 +8499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
@@ -8282,217 +8518,217 @@
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.25" customHeight="1">
-      <c r="B2" s="103" t="s">
+    <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="104" t="s">
+      <c r="K2" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="88" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="107.25" customHeight="1">
-      <c r="B3" s="92" t="s">
+    <row r="3" spans="2:12" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="102" t="s">
+      <c r="I3" s="84"/>
+      <c r="J3" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="126.75" customHeight="1">
-      <c r="B4" s="96" t="s">
+    <row r="4" spans="2:12" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="H4" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="106" t="s">
+      <c r="K4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="100" t="s">
+      <c r="L4" s="83" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="111.75" customHeight="1">
-      <c r="B5" s="92" t="s">
+    <row r="5" spans="2:12" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="83" t="s">
+      <c r="K5" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="112.5" customHeight="1">
-      <c r="B6" s="96" t="s">
+    <row r="6" spans="2:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="99" t="s">
+      <c r="K6" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="100" t="s">
+      <c r="L6" s="83" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="127.5" customHeight="1">
-      <c r="B7" s="92" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="93" t="s">
+    <row r="7" spans="2:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="K7" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="223.5" customHeight="1">
-      <c r="B8" s="89" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="90" t="s">
+    <row r="8" spans="2:12" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="34" t="s">
@@ -8510,59 +8746,59 @@
       <c r="H8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="86" t="s">
+      <c r="I8" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="117.75" customHeight="1">
-      <c r="B9" s="87" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="88" t="s">
+    <row r="9" spans="2:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="106.5" customHeight="1">
-      <c r="B10" s="89" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="90" t="s">
+    <row r="10" spans="2:12" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D10" s="34" t="s">
@@ -8580,59 +8816,59 @@
       <c r="H10" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="100.5" customHeight="1">
-      <c r="B11" s="87" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="88" t="s">
+    <row r="11" spans="2:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="76" t="s">
+      <c r="G11" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="80" t="s">
+      <c r="K11" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="81" t="s">
+      <c r="L11" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="111" customHeight="1">
-      <c r="B12" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="90" t="s">
+    <row r="12" spans="2:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="34" t="s">
@@ -8650,59 +8886,59 @@
       <c r="H12" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="86" t="s">
+      <c r="I12" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="K12" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="131.25" customHeight="1">
-      <c r="B13" s="87" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="88" t="s">
+    <row r="13" spans="2:12" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="80" t="s">
+      <c r="K13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="64" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="118.5" customHeight="1">
-      <c r="B14" s="89" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" s="90" t="s">
+    <row r="14" spans="2:12" ht="118.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="73" t="s">
         <v>91</v>
       </c>
       <c r="D14" s="34" t="s">
@@ -8715,21 +8951,56 @@
         <v>42</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="73" t="s">
+      <c r="K14" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="135.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="57" t="s">
         <v>44</v>
       </c>
     </row>
@@ -8740,116 +9011,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9456DD7-BBEC-42B0-AB3D-1E4232459D96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="58"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="98"/>
       <c r="C3" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="58"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="98"/>
       <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="58"/>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
       <c r="C5" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="58"/>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="98"/>
       <c r="C6" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="58"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="98"/>
       <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="58"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="98"/>
       <c r="C8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="58"/>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="98"/>
       <c r="C9" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B10" s="58"/>
+    <row r="10" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="98"/>
       <c r="C10" s="45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="59"/>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="99"/>
       <c r="C11" s="46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B12" s="55" t="s">
+    <row r="12" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="95" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B13" s="60"/>
+    <row r="13" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="100"/>
       <c r="C13" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B14" s="56"/>
+    <row r="14" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96"/>
       <c r="C14" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="55" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="95" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="96"/>
       <c r="C16" s="44" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B15:B16"/>
@@ -8861,48 +9132,48 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4F0DA6-9A0E-4C2E-8A4F-0A607ED1017F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="26.25" customHeight="1"/>
-    <row r="2" spans="2:3" ht="18" customHeight="1">
-      <c r="B2" s="61" t="s">
+    <row r="1" spans="2:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="101" t="s">
         <v>115</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="62"/>
+    <row r="3" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="102"/>
       <c r="C3" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1">
-      <c r="B4" s="63"/>
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="103"/>
       <c r="C4" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="29.25" customHeight="1">
-      <c r="B5" s="64"/>
+    <row r="5" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="104"/>
       <c r="C5" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="18.75" customHeight="1">
+    <row r="6" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>120</v>
       </c>
@@ -8919,14 +9190,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3699CD-5D7B-4491-8CD4-CAE8F382A34A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
@@ -8935,7 +9206,7 @@
     <col min="6" max="6" width="124.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>25</v>
       </c>
@@ -8952,7 +9223,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="159" customHeight="1">
+    <row r="3" spans="2:6" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41">
         <v>1</v>
       </c>
@@ -8965,7 +9236,7 @@
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="2:6" ht="150" customHeight="1">
+    <row r="4" spans="2:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42">
         <v>2</v>
       </c>
@@ -8978,53 +9249,53 @@
       <c r="E4" s="21"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
     </row>
-    <row r="12" spans="2:6" ht="183" customHeight="1">
-      <c r="B12" s="65" t="s">
+    <row r="12" spans="2:6" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Casos de prueba actualizado durante desarrollo
</commit_message>
<xml_diff>
--- a/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
+++ b/Documentación/PTP_Cristian_Ramirez_Sebastian_Vasquez_260923.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26920"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D80A7C-6B6A-491C-AB30-680F3765FF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Alcance" sheetId="4" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <sheet name="Supuestos" sheetId="11" r:id="rId5"/>
     <sheet name="Bugs" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -410,9 +409,6 @@
     <t>Supongo que todos los prerequisitos estan instalados con las versiones especificadas</t>
   </si>
   <si>
-    <t>Supongo que el equipo entregado cumple con los requisitos mínimos establecidos</t>
-  </si>
-  <si>
     <t>Limitaciones</t>
   </si>
   <si>
@@ -455,12 +451,15 @@
       <t xml:space="preserve"> No se encontraron más bugs. Ya que es una página profesional en producción.</t>
     </r>
   </si>
+  <si>
+    <t>Supongo que el equipo entregado cumple con los requisitos mínimos establecidos.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1345,57 +1344,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1516,9 +1464,60 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1554,7 +1553,7 @@
         <xdr:cNvPr id="12" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,10 +1655,10 @@
         <xdr:cNvPr id="77" name="CuadroTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{C770FEFE-9B8A-D254-21B8-CD22553D21BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1815,10 +1814,10 @@
         <xdr:cNvPr id="26" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4BB75D1E-6C43-46DD-BBBE-50D819C27051}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1974,10 +1973,10 @@
         <xdr:cNvPr id="19" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{E90A3DF6-E11D-4FAC-B9AC-61784C0EE0FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,10 +2155,10 @@
         <xdr:cNvPr id="23" name="CuadroTexto 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{96D281D0-EC22-4202-AC5D-8FCB2D4B5A75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2338,10 +2337,10 @@
         <xdr:cNvPr id="2" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{D9833388-3F32-4994-9C6A-019DE0894BAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2562,10 +2561,10 @@
         <xdr:cNvPr id="41" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{5D8575C3-A739-4016-BC55-112809482EFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2760,10 +2759,10 @@
         <xdr:cNvPr id="15" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{DF603FBC-D3B2-4214-93ED-18C3377F49F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2919,10 +2918,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{72D2F9BC-5088-42CE-A204-0AA8CE025CAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,10 +3090,10 @@
         <xdr:cNvPr id="5" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{9A12C0E9-B04A-4EBE-AB92-459034312EF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3260,10 +3259,10 @@
         <xdr:cNvPr id="16" name="CuadroTexto 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{CA0E62B0-D274-41CD-9443-6BC05777F0FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3445,10 +3444,10 @@
         <xdr:cNvPr id="7" name="CuadroTexto 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F478F35-225A-4862-9470-F9A45447EA8E}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{880432BF-3309-424D-A7E9-DBC52B657E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3630,10 +3629,10 @@
         <xdr:cNvPr id="21" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{978AD3EE-7F52-44AC-A6A5-E8BF0135FDEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3866,10 +3865,10 @@
         <xdr:cNvPr id="75" name="CuadroTexto 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{9F5D409B-744B-227E-6B2E-496CA8237E22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4136,10 +4135,10 @@
         <xdr:cNvPr id="37" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{F67CD31F-0B12-4922-A056-0CC34872AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4436,10 +4435,10 @@
         <xdr:cNvPr id="60" name="CuadroTexto 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{B0BF04F9-D16E-4017-BFFF-6DC56301AD1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5056,10 +5055,10 @@
         <xdr:cNvPr id="42" name="CuadroTexto 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{DCA35E84-9AFF-49B2-A785-FBFFCA78B94A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5326,10 +5325,10 @@
         <xdr:cNvPr id="53" name="CuadroTexto 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{A4732311-C10C-4377-BB9C-7BCBF2FB9364}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5596,10 +5595,10 @@
         <xdr:cNvPr id="55" name="CuadroTexto 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{52376902-504A-4718-9496-42C428C2F961}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5866,10 +5865,10 @@
         <xdr:cNvPr id="72" name="CuadroTexto 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4EF1A362-F3AB-4D90-B111-20D137955FED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6136,10 +6135,10 @@
         <xdr:cNvPr id="43" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{7BF82C8C-C36D-4222-B2B4-C0ED83678A37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6436,10 +6435,10 @@
         <xdr:cNvPr id="64" name="CuadroTexto 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{417FE5B4-E8F5-4E60-A661-D0AE38AA0C55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6736,10 +6735,10 @@
         <xdr:cNvPr id="65" name="CuadroTexto 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{FAF95F8F-79DE-4E7A-BC5C-9F385EFCA522}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7036,10 +7035,10 @@
         <xdr:cNvPr id="73" name="CuadroTexto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D0AEE08-5DD9-499C-A542-BAFB8EE96310}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{3F2EDDDD-D12D-4F0A-B0F3-54C403BAD9FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7341,7 +7340,7 @@
         <xdr:cNvPr id="3" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7385,10 +7384,10 @@
         <xdr:cNvPr id="10" name="CuadroTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{F0D0F3ED-DE82-5F06-8F2C-1F4216EDB65E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7474,10 +7473,10 @@
         <xdr:cNvPr id="2" name="Conector recto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{B524774D-EB98-E422-7C3E-71D0EDC52D04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7532,10 +7531,10 @@
         <xdr:cNvPr id="8" name="CuadroTexto 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{A4E69A13-6422-07C1-BE47-9F38CE90C256}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7731,10 +7730,10 @@
         <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC3E4CBA-057C-6AF1-D775-7E331150DC8D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{021E4413-8A69-4B04-B859-9BDAF4D0FEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7806,7 +7805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -7858,7 +7857,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -8052,27 +8051,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DAC4AF-3F9A-4271-9B0B-277FBE221652}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="23.25" customHeight="1">
+    <row r="2" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8080,60 +8079,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="60.75" customHeight="1">
+    <row r="3" spans="2:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="90" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15" customHeight="1">
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="50"/>
+      <c r="C4" s="90"/>
     </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1">
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="90"/>
     </row>
-    <row r="6" spans="2:3" ht="15" customHeight="1">
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="50"/>
+      <c r="C6" s="90"/>
     </row>
-    <row r="7" spans="2:3" ht="15" customHeight="1">
+    <row r="7" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50"/>
+      <c r="C7" s="90"/>
     </row>
-    <row r="8" spans="2:3" ht="15" customHeight="1">
+    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="C8" s="50"/>
+      <c r="C8" s="90"/>
     </row>
-    <row r="9" spans="2:3" ht="15" customHeight="1">
+    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="50"/>
+      <c r="C9" s="90"/>
     </row>
-    <row r="10" spans="2:3" ht="15" customHeight="1">
+    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="90"/>
     </row>
-    <row r="11" spans="2:3" ht="27.75" customHeight="1">
+    <row r="11" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="91"/>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1"/>
-    <row r="13" spans="2:3" ht="15" customHeight="1"/>
-    <row r="14" spans="2:3" ht="13.5" customHeight="1"/>
-    <row r="15" spans="2:3" ht="15" customHeight="1"/>
-    <row r="16" spans="2:3" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:C11"/>
@@ -8143,113 +8142,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D14B542-D681-42FB-AEEB-27F195955836}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="140.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="53"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="93"/>
       <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="53"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="93"/>
       <c r="C4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B5" s="53"/>
+    <row r="5" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="93"/>
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="53"/>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="93"/>
       <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="53"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="93"/>
       <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="53"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="93"/>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="53"/>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="93"/>
       <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="30" customHeight="1">
-      <c r="B10" s="53"/>
+    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="93"/>
       <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B11" s="53"/>
+    <row r="11" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="93"/>
       <c r="C11" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1">
-      <c r="B12" s="53"/>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="93"/>
       <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="53"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="93"/>
       <c r="C13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="53"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="93"/>
       <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B15" s="53"/>
+    <row r="15" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="93"/>
       <c r="C15" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="16.5" customHeight="1">
-      <c r="B16" s="53"/>
+    <row r="16" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="93"/>
       <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="17.25" customHeight="1">
-      <c r="B17" s="54"/>
+    <row r="17" spans="2:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="94"/>
       <c r="C17" s="16" t="s">
         <v>24</v>
       </c>
@@ -8263,14 +8262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
@@ -8282,217 +8281,217 @@
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="23.25" customHeight="1">
-      <c r="B2" s="103" t="s">
+    <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="104" t="s">
+      <c r="K2" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="88" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="107.25" customHeight="1">
-      <c r="B3" s="92" t="s">
+    <row r="3" spans="2:12" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="94" t="s">
+      <c r="E3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="68" t="s">
+      <c r="F3" s="84"/>
+      <c r="G3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="102" t="s">
+      <c r="I3" s="84"/>
+      <c r="J3" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="126.75" customHeight="1">
-      <c r="B4" s="96" t="s">
+    <row r="4" spans="2:12" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="H4" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="106" t="s">
+      <c r="K4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="100" t="s">
+      <c r="L4" s="83" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="111.75" customHeight="1">
-      <c r="B5" s="92" t="s">
+    <row r="5" spans="2:12" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J5" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="83" t="s">
+      <c r="K5" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="71" t="s">
+      <c r="L5" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="112.5" customHeight="1">
-      <c r="B6" s="96" t="s">
+    <row r="6" spans="2:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="82" t="s">
+      <c r="H6" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="81" t="s">
         <v>42</v>
       </c>
       <c r="J6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="99" t="s">
+      <c r="K6" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="100" t="s">
+      <c r="L6" s="83" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="127.5" customHeight="1">
-      <c r="B7" s="92" t="s">
+    <row r="7" spans="2:12" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="78" t="s">
         <v>42</v>
       </c>
       <c r="J7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="K7" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="223.5" customHeight="1">
-      <c r="B8" s="89" t="s">
+    <row r="8" spans="2:12" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="C8" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="34" t="s">
@@ -8510,59 +8509,59 @@
       <c r="H8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="86" t="s">
+      <c r="I8" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="117.75" customHeight="1">
-      <c r="B9" s="87" t="s">
+    <row r="9" spans="2:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="80" t="s">
+      <c r="K9" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="81" t="s">
+      <c r="L9" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="106.5" customHeight="1">
-      <c r="B10" s="89" t="s">
+    <row r="10" spans="2:12" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D10" s="34" t="s">
@@ -8580,59 +8579,59 @@
       <c r="H10" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="100.5" customHeight="1">
-      <c r="B11" s="87" t="s">
+    <row r="11" spans="2:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="76" t="s">
+      <c r="G11" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="80" t="s">
+      <c r="K11" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="81" t="s">
+      <c r="L11" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="111" customHeight="1">
-      <c r="B12" s="89" t="s">
+    <row r="12" spans="2:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="73" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="34" t="s">
@@ -8650,59 +8649,59 @@
       <c r="H12" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="86" t="s">
+      <c r="I12" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="K12" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="131.25" customHeight="1">
-      <c r="B13" s="87" t="s">
+    <row r="13" spans="2:12" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="68" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="80" t="s">
+      <c r="K13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="81" t="s">
+      <c r="L13" s="64" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="118.5" customHeight="1">
-      <c r="B14" s="89" t="s">
+    <row r="14" spans="2:12" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="73" t="s">
         <v>91</v>
       </c>
       <c r="D14" s="34" t="s">
@@ -8720,16 +8719,16 @@
       <c r="H14" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="86" t="s">
+      <c r="I14" s="69" t="s">
         <v>42</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="73" t="s">
+      <c r="K14" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="57" t="s">
         <v>44</v>
       </c>
     </row>
@@ -8740,116 +8739,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9456DD7-BBEC-42B0-AB3D-1E4232459D96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="58"/>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="98"/>
       <c r="C3" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="58"/>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="98"/>
       <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="58"/>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
       <c r="C5" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="58"/>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="98"/>
       <c r="C6" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="58"/>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="98"/>
       <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="58"/>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="98"/>
       <c r="C8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="58"/>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="98"/>
       <c r="C9" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B10" s="58"/>
+    <row r="10" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="98"/>
       <c r="C10" s="45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="59"/>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="99"/>
       <c r="C11" s="46" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B12" s="55" t="s">
+    <row r="12" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="95" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B13" s="60"/>
+    <row r="13" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="100"/>
       <c r="C13" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B14" s="56"/>
+    <row r="14" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="96"/>
       <c r="C14" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="55" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="95" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="56"/>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="96"/>
       <c r="C16" s="44" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B15:B16"/>
@@ -8861,53 +8860,53 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4F0DA6-9A0E-4C2E-8A4F-0A607ED1017F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="26.25" customHeight="1"/>
-    <row r="2" spans="2:3" ht="18" customHeight="1">
-      <c r="B2" s="61" t="s">
+    <row r="1" spans="2:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="101" t="s">
         <v>115</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="62"/>
+    <row r="3" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="102"/>
       <c r="C3" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.75" customHeight="1">
-      <c r="B4" s="63"/>
+    <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="103"/>
       <c r="C4" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="29.25" customHeight="1">
-      <c r="B5" s="64"/>
+    <row r="5" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="104"/>
       <c r="C5" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="18.75" customHeight="1">
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="47" t="s">
         <v>120</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -8919,14 +8918,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3699CD-5D7B-4491-8CD4-CAE8F382A34A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
@@ -8935,24 +8934,24 @@
     <col min="6" max="6" width="124.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75">
+    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>124</v>
-      </c>
     </row>
-    <row r="3" spans="2:6" ht="159" customHeight="1">
+    <row r="3" spans="2:6" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41">
         <v>1</v>
       </c>
@@ -8960,71 +8959,71 @@
         <v>65</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="2:6" ht="150" customHeight="1">
+    <row r="4" spans="2:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="42">
         <v>2</v>
       </c>
       <c r="C4" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>126</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>127</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
     </row>
-    <row r="12" spans="2:6" ht="183" customHeight="1">
-      <c r="B12" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="66"/>
+    <row r="12" spans="2:6" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="105" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>